<commit_message>
resultados obtidos - SUS
</commit_message>
<xml_diff>
--- a/respostas_questionario/avaliacao_sus.xlsx
+++ b/respostas_questionario/avaliacao_sus.xlsx
@@ -178,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -186,6 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,35 +467,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -511,10 +514,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -533,8 +539,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -545,16 +554,19 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -562,10 +574,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
         <v>3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -573,8 +585,11 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -582,19 +597,22 @@
         <v>14</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="E6" s="1">
-        <v>4</v>
-      </c>
       <c r="F6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -613,8 +631,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -622,19 +643,22 @@
         <v>16</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -642,19 +666,22 @@
         <v>17</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -662,19 +689,22 @@
         <v>18</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
         <v>5</v>
       </c>
       <c r="E10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -682,41 +712,47 @@
         <v>19</v>
       </c>
       <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="D12" s="4">
         <v>90</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>82.5</v>
-      </c>
-      <c r="E12" s="4">
-        <v>90</v>
       </c>
       <c r="F12" s="4">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
+      <c r="G12" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="6">
         <v>88.125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sus final na tese
</commit_message>
<xml_diff>
--- a/respostas_questionario/avaliacao_sus.xlsx
+++ b/respostas_questionario/avaliacao_sus.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6960" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="SUS Prototipo" sheetId="1" r:id="rId1"/>
+    <sheet name="SUS HMI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>I think that I would like to use this system frequently.</t>
   </si>
@@ -102,13 +103,25 @@
   </si>
   <si>
     <t>Score Final</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +137,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +168,11 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -175,10 +200,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -187,8 +213,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Correto" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,4 +788,432 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="8">
+        <v>4</v>
+      </c>
+      <c r="K2" s="8">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8">
+        <v>5</v>
+      </c>
+      <c r="M2" s="8">
+        <v>1</v>
+      </c>
+      <c r="N2" s="8">
+        <v>4</v>
+      </c>
+      <c r="O2" s="8">
+        <v>1</v>
+      </c>
+      <c r="P2" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>2</v>
+      </c>
+      <c r="R2" s="8">
+        <v>4</v>
+      </c>
+      <c r="S2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="8">
+        <v>4</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
+        <v>5</v>
+      </c>
+      <c r="M3" s="8">
+        <v>2</v>
+      </c>
+      <c r="N3" s="8">
+        <v>5</v>
+      </c>
+      <c r="O3" s="8">
+        <v>1</v>
+      </c>
+      <c r="P3" s="8">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>1</v>
+      </c>
+      <c r="R3" s="8">
+        <v>5</v>
+      </c>
+      <c r="S3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="D12" s="4">
+        <v>92.5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>87.5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>90</v>
+      </c>
+      <c r="G12" s="4">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="6">
+        <v>89.375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>